<commit_message>
last commit before soutenance
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Catégorie</t>
   </si>
@@ -39,122 +39,137 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>Balises description et title</t>
-  </si>
-  <si>
-    <t>Balises non compléte</t>
-  </si>
-  <si>
-    <t>Liens inutiles footer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liens </t>
-  </si>
-  <si>
-    <t>Liens externe coohérent et propre</t>
-  </si>
-  <si>
-    <t>MAJ biblio</t>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Contrast Errors</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Accessibilit%C3%A9/Checklist_accessibilite_mobile</t>
+  </si>
+  <si>
+    <t>Un contraste dont le ratio est de 4.5:1 pour les textes normaux (dont la fonte est inférieure à 18 points ou 14 points en gras) ; Un contraste dont le ratio est de 3:1 pour les grands textes (18 points minimum ou 14 points en gras).</t>
+  </si>
+  <si>
+    <t>L'accessibilité des couleurs se mesurent notamment par le contraste entre la couleur du texte et sa couleur de fond. Il y a un certain ratio à respecter afin d'assurer une bonne lisibilité du texte par des personnes malvoyantes.</t>
+  </si>
+  <si>
+    <t>Language missing or invalid</t>
+  </si>
+  <si>
+    <t>Strutural Elements</t>
+  </si>
+  <si>
+    <t>Accessibilité et Performance</t>
+  </si>
+  <si>
+    <t>https://blog.yabawt.com/marketing/comment-bien-structurer-vos-pages-pour-le-seo/</t>
+  </si>
+  <si>
+    <t>Identifier le langage de votre contenu vous permet d'effectuer plusieurs tâches automatiquement, du changement de l'apparence de votre page à l'extraction d'informations ou à la modification du fonctionnement d'une application. Certaines applications de langage fonctionnent sur l'ensemble du document, d'autres sur des parties du document convenablement étiquetées.</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-lang-why.fr#:~:text=Pourquoi%20dois%2Dje%20utiliser%20l,du%20texte%20sur%20la%20page.</t>
+  </si>
+  <si>
+    <t>L'attribut HTML lang peut être utilisée pour déclarer la langue d'une page Web ou d'une partie d'une page Web. Le but est d'aider les moteurs de recherche et les navigateurs.</t>
+  </si>
+  <si>
+    <t>Le H1 est un Hn particulier. En effet, pour un moteur de recherche, il ne doit apparaître qu’une fois dans votre page. Viennent ensuite les autres Hn, du H2 au H6. Pour commencer, nous vous conseillons de vous limiter aux H2 et aux H3 autant que faire se peut, sauf cas exceptionnel (contenu particulièrement long, sous-partie indispensable…), et de ne jamais dépasser le niveau H4.</t>
   </si>
   <si>
     <t>SEO</t>
   </si>
   <si>
-    <t>Accessibility</t>
-  </si>
-  <si>
-    <t>Best pratice</t>
-  </si>
-  <si>
-    <t>Probleme securité et performance</t>
-  </si>
-  <si>
-    <t>Texte dans img</t>
-  </si>
-  <si>
-    <t>Les textes dans les images ne sont pas identifiers par google bots</t>
-  </si>
-  <si>
-    <t>Mise en page du texte dans des balises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balise lang </t>
-  </si>
-  <si>
-    <t>Aucune langue préciser</t>
-  </si>
-  <si>
-    <t>Ajout du "fr" dans la balise lang</t>
-  </si>
-  <si>
-    <t>Couleur contrast</t>
-  </si>
-  <si>
-    <t>Les contrast ne sont pas correct pour une visibilité parfaite</t>
-  </si>
-  <si>
-    <t>Demande au graphiste de modifier ca</t>
-  </si>
-  <si>
-    <t>Refonte du site</t>
+    <t>Document does not have a meta description</t>
+  </si>
+  <si>
+    <t>Document have a title empty</t>
+  </si>
+  <si>
+    <t>Ce title est particulièrement important en SEO. D’abord car ce sont les premiers mots que les internautes verront de votre page, ce sont donc eux qui donneront ou non envie de cliquer pour consulter votre site. Ensuite parce que la balise &lt;title&gt; est largement utilisée par Google pour référencer les pages web. Ne pas renseigner de title ou renseigner un title de mauvaise qualité, c’est donc se tirer une balle dans le pied d’un point de vue SEO.</t>
+  </si>
+  <si>
+    <t>En effet, title et méta description se complètent. La méta description apparait sur les SERP, juste en dessous du title. L’un ne va donc pas sans l’autre.</t>
+  </si>
+  <si>
+    <t>En effet, vous devez faire apparaître votre mot-clé dans votre title ainsi que dans votre méta description, c’est la base. Vous pouvez également y ajouter le nom de votre marque, c’est toujours utile. Mais ce n’est pas tout ! Car pour que vos méta-informations s’affichent correctement sur les SERP et soient efficaces pour votre SEO, elles doivent respecter des contraintes de longueur. Title entre 40 et 60 caractères et la meta description entre 140 et 150 caractères</t>
+  </si>
+  <si>
+    <t>Réduire la qualité de l’image peut accélérer la vitesse de chargement d’un site Web. Les sites Web rapides signifient une meilleure expérience utilisateur, ce qui entraîne une augmentation des conversions. Selon une étude de Kissmetrics, un délai d’une seconde en réponse à une page peut entraîner une réduction de 7% des conversions.</t>
+  </si>
+  <si>
+    <t>Perfomance</t>
+  </si>
+  <si>
+    <t>Properly size and optimized images</t>
+  </si>
+  <si>
+    <t>Les images trop lourdes ralentisses la vitesse de chargement du site et devient une contrainte pour l'utilisateur.</t>
+  </si>
+  <si>
+    <t>https://yesyouweb.com/pourquoi-comment-optimiser-images-site-web/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibilité </t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Son utilisation permet aux navigateurs d’associer cet intitulé au champ de formulaire. Ainsi, un clic sur l’intitulé donnera le focus au champs de formulaire, ce qui est très pratique par exemple pour les boutons radio ou cases à cocher parfois trop petites pour certains utilisateurs. Ce mécanisme est important également pour les lecteurs d’écran, qui ont besoin d'étiquettes explicites pour associer chaque champ de formulaire à un texte.</t>
+  </si>
+  <si>
+    <t>Pour que le label soit explicite, il faut utiliser les attributs for (sur l’élément label) et id (sur le champ de formulaire) avec la même valeur.</t>
   </si>
   <si>
     <t>Performance</t>
   </si>
   <si>
-    <t>Tailles images</t>
-  </si>
-  <si>
-    <t>Images trop lourdes et grandes</t>
-  </si>
-  <si>
-    <t>Resize des images et optimisation du poid</t>
-  </si>
-  <si>
-    <t>Alt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alt sur les images incorrectes </t>
-  </si>
-  <si>
-    <t>Réécriture des alt</t>
-  </si>
-  <si>
-    <t>width et height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Largeur et hauteur des images non precisé </t>
-  </si>
-  <si>
-    <t>ajout width et height sur les balises img</t>
-  </si>
-  <si>
-    <t>Texte coohérent et propre</t>
-  </si>
-  <si>
-    <t>Aria label</t>
-  </si>
-  <si>
-    <t>Lien extérieur non identifier</t>
-  </si>
-  <si>
-    <t>ajout de la classe "aria-label" pour identifier les liens sortant "reseaux sociaux"</t>
-  </si>
-  <si>
-    <t>Meta name Keywords</t>
-  </si>
-  <si>
-    <t>Répétition des mots clés abusives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faire un brainstorming avec l'équipe pour trouver des mots clés pertinents </t>
+    <t>CDN</t>
+  </si>
+  <si>
+    <t>Réduire le temps de téléchargement : les fichiers utilisés par plusieurs sites utilisant le même CDN ne seront téléchargés qu’une seule fois. Ensuite ils seront placés dans le cache, ce qui évite de les retélécharger. Cela est d’autant plus vrai pour les bibliothèques couramment utilisées telles que jQuery, Bootstrap, FontAwesome, etc.</t>
+  </si>
+  <si>
+    <t>Le temps de chargement d’une page est un critère important pour l’utilisateur. Pour accélérer celui-ci les CDN (Content Delivery Network) proposent d’héberger les fichiers statiques (CSS, JS, Images) sur leurs serveurs.</t>
+  </si>
+  <si>
+    <t>https://www.softfluent.fr/blog/to-cdn-or-not-to-cdn-pourquoi-choisir/</t>
+  </si>
+  <si>
+    <t>Les titres doivent apparaitrent en texte propre et non en image pour amérioler le site en Performance, SEO et accessibilité.</t>
+  </si>
+  <si>
+    <t>ALT</t>
+  </si>
+  <si>
+    <t>Dans la balise ALT de votre image, ne vous contentez pas d’écrire un mot pour définir ce qu’elle représente. Il est effectivement question de positionner dans cette balise une description précise de l’image.</t>
+  </si>
+  <si>
+    <t>Fut un temps où la mode était au bourrage de mots-clés dans la balise ALT. Autrement dit, cette dernière pouvait ressembler à cela : " La chouette agence, agence web paris, création logo paris". Sachez qu’une telle pratique est aujourd’hui à bannir.</t>
+  </si>
+  <si>
+    <t>https://www.redacteur.com/blog/seo-balise-alt-images/#:~:text=En%20effet%2C%20le%20texte%20alternatif,aussi%20au%20r%C3%A9f%C3%A9rencement%20par%20image.</t>
+  </si>
+  <si>
+    <t>Document does not use legible font size</t>
+  </si>
+  <si>
+    <t>Le « content cloaking » ou la dissimulation de contenu sur un site web est l’une des plus anciennes tactiques SEO. Lorsque les moteurs de recherche étaient moins sophistiqués, cacher des mots-clés et liens permettait d’obtenir un meilleur classement. Aujourd’hui cette technique appartient aux Black Hat.</t>
+  </si>
+  <si>
+    <t>Il s’agit ici de la technique la plus “sale” et la plus risquée. Elle consiste simplement à ajouter du texte invisible (par exemple écrit en blanc sur fond blanc) et de le disséminer un peu partout dans la page. Si cela fonctionnait très bien il y a 10 ou 15 ans, c’est aujourd’hui une méthode révolue qu’il faut absolument proscrire. Google sait très bien repérer ces textes cachés. Pour optimiser votre référencement naturel, il vaut donc mieux opter pour un texte entièrement visible </t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-technique-seo-cloaking/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -174,10 +189,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -185,6 +196,30 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -218,35 +253,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,19 +510,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="26" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="47.44140625" customWidth="1"/>
+    <col min="4" max="4" width="44.21875" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="37.88671875" customWidth="1"/>
+    <col min="8" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -507,241 +568,248 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" ht="75">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="105">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:26" ht="120">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:26" ht="120">
+      <c r="A5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:26" ht="45">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:26" ht="105">
+      <c r="A7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="135">
+      <c r="A8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="105">
+      <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="90">
+      <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="30">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6"/>
+    <row r="11" spans="1:26" ht="135">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="45">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" ht="30">
-      <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" ht="30">
-      <c r="A6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="30">
-      <c r="A7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" ht="60">
-      <c r="A8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" ht="45">
-      <c r="A9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" ht="30">
-      <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" ht="30">
-      <c r="A11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" ht="45">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6"/>
+    <row r="12" spans="1:26" ht="15.75">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="15.75">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="15.75">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="15.75">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="15.75">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+    </row>
     <row r="27" ht="15.75" customHeight="1"/>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1"/>
@@ -1716,8 +1784,17 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D5:D6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2"/>
+    <hyperlink ref="F6" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>